<commit_message>
Adição dos resultados e correção de alguns gráficos
</commit_message>
<xml_diff>
--- a/calculos.xlsx
+++ b/calculos.xlsx
@@ -1,6 +1,6 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26026"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Projetos\LabExperimentacao\medicao-lab1\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{FD97B4F7-4230-448C-ADFF-343F351363D4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CE59D2E4-2FDC-466A-9A9A-25B287F11654}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1"/>
+    <workbookView xWindow="22932" yWindow="-108" windowWidth="23256" windowHeight="13176" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="calculos" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,20 @@
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">calculos!$F$2:$F$1001</definedName>
     <definedName name="_xlnm.Extract" localSheetId="0">analise!$J$59</definedName>
   </definedNames>
-  <calcPr calcId="0"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
@@ -3297,7 +3310,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.0000"/>
   </numFmts>
@@ -3801,7 +3814,7 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -3822,7 +3835,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Ênfase1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -4102,7 +4114,6 @@
           </c:extLst>
         </c:ser>
         <c:dLbls>
-          <c:dLblPos val="outEnd"/>
           <c:showLegendKey val="0"/>
           <c:showVal val="0"/>
           <c:showCatName val="0"/>
@@ -4194,7 +4205,7 @@
           <a:effectLst/>
         </c:spPr>
         <c:txPr>
-          <a:bodyPr rot="5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:bodyPr rot="5400000" spcFirstLastPara="1" vertOverflow="ellipsis" wrap="square" anchor="ctr" anchorCtr="1"/>
           <a:lstStyle/>
           <a:p>
             <a:pPr>
@@ -5573,8 +5584,13 @@
                 </a:pPr>
                 <a:r>
                   <a:rPr lang="pt-BR"/>
-                  <a:t>Média de Releases/Mês</a:t>
+                  <a:t>Tempo da Última</a:t>
                 </a:r>
+                <a:r>
+                  <a:rPr lang="pt-BR" baseline="0"/>
+                  <a:t> Atualização (dias)</a:t>
+                </a:r>
+                <a:endParaRPr lang="pt-BR"/>
               </a:p>
             </c:rich>
           </c:tx>
@@ -5853,7 +5869,7 @@
             </a:r>
             <a:r>
               <a:rPr lang="en-US" b="1" baseline="0"/>
-              <a:t> 5 - </a:t>
+              <a:t> 6 - </a:t>
             </a:r>
             <a:r>
               <a:rPr lang="en-US" b="1"/>
@@ -5861,7 +5877,7 @@
             </a:r>
             <a:r>
               <a:rPr lang="en-US" b="1" baseline="0"/>
-              <a:t> de Tempo da Última Atualização</a:t>
+              <a:t> de % de Issues Fechadas</a:t>
             </a:r>
             <a:endParaRPr lang="en-US" b="1"/>
           </a:p>
@@ -5972,34 +5988,34 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="10"/>
                 <c:pt idx="0">
-                  <c:v>421</c:v>
+                  <c:v>54</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>55</c:v>
+                  <c:v>7</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>58</c:v>
+                  <c:v>14</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>52</c:v>
+                  <c:v>33</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>28</c:v>
+                  <c:v>34</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>33</c:v>
+                  <c:v>47</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>33</c:v>
+                  <c:v>78</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>21</c:v>
+                  <c:v>116</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>34</c:v>
+                  <c:v>206</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>14</c:v>
+                  <c:v>416</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -9495,11 +9511,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:M1001"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="M1001" sqref="M1001"/>
+    <sheetView topLeftCell="A25" workbookViewId="0">
+      <selection activeCell="M2" sqref="M2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -51228,11 +51244,11 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A2:U71"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L78" sqref="L78"/>
+    <sheetView tabSelected="1" topLeftCell="J43" workbookViewId="0">
+      <selection activeCell="U67" sqref="U67"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -51794,6 +51810,10 @@
         <f>COUNTIFS(calculos!$I$2:$I$1001,"&gt;"&amp;analise!A14,calculos!$I$2:$I$1001,"&lt;="&amp;analise!B14)</f>
         <v>58</v>
       </c>
+      <c r="F14">
+        <f>690/1000</f>
+        <v>0.69</v>
+      </c>
       <c r="H14">
         <f t="shared" si="2"/>
         <v>135000</v>
@@ -51979,8 +51999,8 @@
         <v>Até 10</v>
       </c>
       <c r="S45" s="3">
-        <f>COUNTIFS(calculos!$K$2:$K$1001,"&gt;="&amp;analise!P45,calculos!$K$2:$K$1001,"&lt;="&amp;analise!Q45)</f>
-        <v>421</v>
+        <f>COUNTIFS(calculos!$M$2:$M$1001,"&gt;="&amp;analise!P45,calculos!$M$2:$M$1001,"&lt;="&amp;analise!Q45)</f>
+        <v>54</v>
       </c>
     </row>
     <row r="46" spans="1:21" x14ac:dyDescent="0.25">
@@ -52036,8 +52056,8 @@
         <v>Entre 10 e 20</v>
       </c>
       <c r="S46" s="3">
-        <f>COUNTIFS(calculos!$K$2:$K$1001,"&gt;="&amp;analise!P46,calculos!$K$2:$K$1001,"&lt;="&amp;analise!Q46)</f>
-        <v>55</v>
+        <f>COUNTIFS(calculos!$M$2:$M$1001,"&gt;="&amp;analise!P46,calculos!$M$2:$M$1001,"&lt;="&amp;analise!Q46)</f>
+        <v>7</v>
       </c>
     </row>
     <row r="47" spans="1:21" x14ac:dyDescent="0.25">
@@ -52093,8 +52113,8 @@
         <v>Entre 20 e 30</v>
       </c>
       <c r="S47" s="3">
-        <f>COUNTIFS(calculos!$K$2:$K$1001,"&gt;="&amp;analise!P47,calculos!$K$2:$K$1001,"&lt;="&amp;analise!Q47)</f>
-        <v>58</v>
+        <f>COUNTIFS(calculos!$M$2:$M$1001,"&gt;="&amp;analise!P47,calculos!$M$2:$M$1001,"&lt;="&amp;analise!Q47)</f>
+        <v>14</v>
       </c>
     </row>
     <row r="48" spans="1:21" x14ac:dyDescent="0.25">
@@ -52164,14 +52184,14 @@
         <v>Entre 30 e 40</v>
       </c>
       <c r="S48" s="3">
-        <f>COUNTIFS(calculos!$K$2:$K$1001,"&gt;="&amp;analise!P48,calculos!$K$2:$K$1001,"&lt;="&amp;analise!Q48)</f>
-        <v>52</v>
+        <f>COUNTIFS(calculos!$M$2:$M$1001,"&gt;="&amp;analise!P48,calculos!$M$2:$M$1001,"&lt;="&amp;analise!Q48)</f>
+        <v>33</v>
       </c>
       <c r="T48" t="s">
         <v>1073</v>
       </c>
       <c r="U48" s="9">
-        <f>AVERAGE(calculos!M2:M1001)</f>
+        <f>AVERAGE(calculos!$M$2:$M$1001)</f>
         <v>0.76779589816665428</v>
       </c>
     </row>
@@ -52242,8 +52262,8 @@
         <v>Entre 40 e 50</v>
       </c>
       <c r="S49" s="3">
-        <f>COUNTIFS(calculos!$K$2:$K$1001,"&gt;="&amp;analise!P49,calculos!$K$2:$K$1001,"&lt;="&amp;analise!Q49)</f>
-        <v>28</v>
+        <f>COUNTIFS(calculos!$M$2:$M$1001,"&gt;="&amp;analise!P49,calculos!$M$2:$M$1001,"&lt;="&amp;analise!Q49)</f>
+        <v>34</v>
       </c>
       <c r="T49" t="s">
         <v>1074</v>
@@ -52306,8 +52326,8 @@
         <v>Entre 50 e 60</v>
       </c>
       <c r="S50" s="3">
-        <f>COUNTIFS(calculos!$K$2:$K$1001,"&gt;="&amp;analise!P50,calculos!$K$2:$K$1001,"&lt;="&amp;analise!Q50)</f>
-        <v>33</v>
+        <f>COUNTIFS(calculos!$M$2:$M$1001,"&gt;="&amp;analise!P50,calculos!$M$2:$M$1001,"&lt;="&amp;analise!Q50)</f>
+        <v>47</v>
       </c>
     </row>
     <row r="51" spans="1:21" x14ac:dyDescent="0.25">
@@ -52377,8 +52397,8 @@
         <v>Entre 60 e 70</v>
       </c>
       <c r="S51" s="3">
-        <f>COUNTIFS(calculos!$K$2:$K$1001,"&gt;="&amp;analise!P51,calculos!$K$2:$K$1001,"&lt;="&amp;analise!Q51)</f>
-        <v>33</v>
+        <f>COUNTIFS(calculos!$M$2:$M$1001,"&gt;="&amp;analise!P51,calculos!$M$2:$M$1001,"&lt;="&amp;analise!Q51)</f>
+        <v>78</v>
       </c>
     </row>
     <row r="52" spans="1:21" x14ac:dyDescent="0.25">
@@ -52434,8 +52454,8 @@
         <v>Entre 70 e 80</v>
       </c>
       <c r="S52" s="3">
-        <f>COUNTIFS(calculos!$K$2:$K$1001,"&gt;="&amp;analise!P52,calculos!$K$2:$K$1001,"&lt;="&amp;analise!Q52)</f>
-        <v>21</v>
+        <f>COUNTIFS(calculos!$M$2:$M$1001,"&gt;="&amp;analise!P52,calculos!$M$2:$M$1001,"&lt;="&amp;analise!Q52)</f>
+        <v>116</v>
       </c>
       <c r="T52" t="s">
         <v>1086</v>
@@ -52499,8 +52519,8 @@
         <v>Entre 80 e 90</v>
       </c>
       <c r="S53" s="3">
-        <f>COUNTIFS(calculos!$K$2:$K$1001,"&gt;="&amp;analise!P53,calculos!$K$2:$K$1001,"&lt;="&amp;analise!Q53)</f>
-        <v>34</v>
+        <f>COUNTIFS(calculos!$M$2:$M$1001,"&gt;="&amp;analise!P53,calculos!$M$2:$M$1001,"&lt;="&amp;analise!Q53)</f>
+        <v>206</v>
       </c>
     </row>
     <row r="54" spans="1:21" x14ac:dyDescent="0.25">
@@ -52556,8 +52576,8 @@
         <v>Entre 90 e 100</v>
       </c>
       <c r="S54" s="3">
-        <f>COUNTIFS(calculos!$K$2:$K$1001,"&gt;="&amp;analise!P54,calculos!$K$2:$K$1001,"&lt;="&amp;analise!Q54)</f>
-        <v>14</v>
+        <f>COUNTIFS(calculos!$M$2:$M$1001,"&gt;="&amp;analise!P54,calculos!$M$2:$M$1001,"&lt;="&amp;analise!Q54)</f>
+        <v>416</v>
       </c>
     </row>
     <row r="55" spans="1:21" x14ac:dyDescent="0.25">
@@ -52571,9 +52591,6 @@
     </row>
     <row r="58" spans="1:21" x14ac:dyDescent="0.25">
       <c r="K58" s="6"/>
-    </row>
-    <row r="60" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="N60" s="10"/>
     </row>
     <row r="71" spans="13:13" x14ac:dyDescent="0.25">
       <c r="M71" s="6"/>

</xml_diff>